<commit_message>
Problem 3: Gun Violence
</commit_message>
<xml_diff>
--- a/homework/hw1/data/immigration_census_data.xlsx
+++ b/homework/hw1/data/immigration_census_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reece/Desktop/math4334/homework/hw1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DC5115-622B-3643-B07D-0C2FD1F5C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B0717E-E815-684B-A3FF-049172601AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17380" xr2:uid="{3CDAE095-66CB-814C-8391-E71DCFEA5AF9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17460" xr2:uid="{3CDAE095-66CB-814C-8391-E71DCFEA5AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,11 +610,14 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>